<commit_message>
Add log4j logger & implementation
</commit_message>
<xml_diff>
--- a/testData/UserData.xlsx
+++ b/testData/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hen Benoish\Documents\GitHub\MyPetStoreAPITesting\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D1E02E-418C-4131-909F-C73BEA809862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F6E84E-E9F0-40C7-AFAD-A91ACE28D5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>username</t>
   </si>
@@ -40,9 +40,6 @@
     <t>phone</t>
   </si>
   <si>
-    <t>user_5</t>
-  </si>
-  <si>
     <t>user_4</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>user_2</t>
   </si>
   <si>
-    <t>user_9</t>
-  </si>
-  <si>
     <t>Michael</t>
   </si>
   <si>
@@ -64,15 +58,6 @@
     <t>Sophia</t>
   </si>
   <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Olivia</t>
-  </si>
-  <si>
     <t>Miller</t>
   </si>
   <si>
@@ -85,12 +70,6 @@
     <t>Jones</t>
   </si>
   <si>
-    <t>Wilson</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>michael.miller@gmail.com</t>
   </si>
   <si>
@@ -103,21 +82,6 @@
     <t>michael.jones@example.com</t>
   </si>
   <si>
-    <t>jane.miller@example.com</t>
-  </si>
-  <si>
-    <t>john.davis@gmail.com</t>
-  </si>
-  <si>
-    <t>michael.wilson@yahoo.com</t>
-  </si>
-  <si>
-    <t>jane.davis@outlook.com</t>
-  </si>
-  <si>
-    <t>olivia.smith@example.com</t>
-  </si>
-  <si>
     <t>pass123</t>
   </si>
   <si>
@@ -127,9 +91,6 @@
     <t>letmein</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
     <t>123-456-7890</t>
   </si>
   <si>
@@ -139,25 +100,10 @@
     <t>987-654-3210</t>
   </si>
   <si>
-    <t>111-222-3333</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>user_1</t>
-  </si>
-  <si>
-    <t>user_6</t>
-  </si>
-  <si>
-    <t>user_7</t>
-  </si>
-  <si>
-    <t>user_8</t>
-  </si>
-  <si>
-    <t>user_10</t>
   </si>
 </sst>
 </file>
@@ -549,26 +495,69 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2F1D56D1-D817-447F-A067-66F665CB7809}">
+  <we:reference id="wa200005502" version="1.0.0.5" store="he-IL" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200005502" version="1.0.0.5" store="WA200005502" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="docId" value="&quot;b914b1cb-2061-4da6-adc1-2ca12a20b483&quot;"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_GPT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_HLIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_CLASSIFY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TRANSLATE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_EXTRACT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TAG</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_CONVERT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_FORMAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_SUMMARIZE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TABLE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_FILL</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -589,234 +578,96 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45616</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>77665</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>74576</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45365</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>44455</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6547</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>87566</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>346534</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>3344223</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1122342</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>